<commit_message>
Updated models for experiment 1 and changed the text location.
</commit_message>
<xml_diff>
--- a/Data/frequencies_exp1_and_lago.xlsx
+++ b/Data/frequencies_exp1_and_lago.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">n1</t>
   </si>
   <si>
-    <t xml:space="preserve">lago</t>
+    <t xml:space="preserve">lagoetal</t>
   </si>
   <si>
     <t xml:space="preserve">-0.512591016</t>
@@ -766,7 +766,7 @@
     <t xml:space="preserve">yönetici</t>
   </si>
   <si>
-    <t xml:space="preserve">up</t>
+    <t xml:space="preserve">exp1</t>
   </si>
   <si>
     <t xml:space="preserve">0.151940891</t>
@@ -1420,8 +1420,8 @@
   </sheetPr>
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K90" activeCellId="0" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>